<commit_message>
new gel rig post
</commit_message>
<xml_diff>
--- a/images/mtORF PCR Template.xlsx
+++ b/images/mtORF PCR Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Putnam_Lab_Notebook/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B8D4D6-932A-0B43-81CE-011FCB2C8A06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDB30DC-CF63-B247-BB9A-2877A6AD66E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67200" yWindow="3840" windowWidth="28800" windowHeight="13920" xr2:uid="{1D54ADAE-84BE-3A4D-A3DA-CF53576EBF26}"/>
+    <workbookView xWindow="0" yWindow="2920" windowWidth="28800" windowHeight="13920" xr2:uid="{1D54ADAE-84BE-3A4D-A3DA-CF53576EBF26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>